<commit_message>
voor maken nieuwe cohorten
</commit_message>
<xml_diff>
--- a/public/cohort/fileExcel/EC PTA en onderwijsprogramma.xlsx
+++ b/public/cohort/fileExcel/EC PTA en onderwijsprogramma.xlsx
@@ -1,16 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23929"/>
   <fileSharing userName="Schadenberg, K." algorithmName="SHA-512" hashValue="/RtgpqBn4CVbkxG4MgE4aovhv9a74c6BZIvWdYv2qH3z7/l3E8lEpafXxhj+1Ob1fvwjjMZygVJuD9Mc4Id/1Q==" saltValue="wHVogFwvQQ7FVXHFJxtlHQ==" spinCount="100000"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csgnl.sharepoint.com/teams/AUG-mdw/Shared Documents/Toetsing/PTA en PTB bovenbouw 20-21/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:10000_{199A9C43-AB1C-418C-92B1-EE3747959307}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="800" firstSheet="1" activeTab="6"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="800" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Instellingen" sheetId="3" r:id="rId1"/>
@@ -21,22 +22,12 @@
     <sheet name="5A PTA en programma" sheetId="11" r:id="rId6"/>
     <sheet name="6A PTA en programma" sheetId="12" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="129">
   <si>
     <t>Vakken</t>
   </si>
@@ -348,9 +339,6 @@
   </si>
   <si>
     <t>Lesbrieven: Marktgedrag, Mobiliteit.</t>
-  </si>
-  <si>
-    <t>nee</t>
   </si>
   <si>
     <t>Boek Pincode: hoofdstuk 3 en 4 Arbeid</t>
@@ -431,7 +419,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -970,21 +958,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView zoomScale="25" zoomScaleNormal="25" workbookViewId="0">
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.109375" style="14"/>
-    <col min="3" max="3" width="15.44140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.109375" style="14"/>
+    <col min="1" max="2" width="9.140625" style="14"/>
+    <col min="3" max="3" width="15.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1001,7 +989,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>5</v>
       </c>
@@ -1024,7 +1012,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>10</v>
       </c>
@@ -1047,7 +1035,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>15</v>
       </c>
@@ -1067,7 +1055,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>20</v>
       </c>
@@ -1087,7 +1075,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>25</v>
       </c>
@@ -1101,7 +1089,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>29</v>
       </c>
@@ -1112,7 +1100,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="14" t="s">
         <v>22</v>
       </c>
@@ -1123,7 +1111,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" s="14" t="s">
         <v>17</v>
       </c>
@@ -1134,7 +1122,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" s="14" t="s">
         <v>35</v>
       </c>
@@ -1145,7 +1133,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
         <v>38</v>
       </c>
@@ -1156,7 +1144,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="14" t="s">
         <v>41</v>
       </c>
@@ -1167,7 +1155,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
         <v>44</v>
       </c>
@@ -1178,7 +1166,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="14" t="s">
         <v>30</v>
       </c>
@@ -1189,7 +1177,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="14" t="s">
         <v>47</v>
       </c>
@@ -1200,7 +1188,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="E16" s="14" t="s">
         <v>49</v>
       </c>
@@ -1208,7 +1196,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E17" s="14" t="s">
         <v>38</v>
       </c>
@@ -1216,7 +1204,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="18" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E18" s="14" t="s">
         <v>52</v>
       </c>
@@ -1224,7 +1212,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="19" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E19" s="14" t="s">
         <v>54</v>
       </c>
@@ -1232,7 +1220,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="20" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E20" s="14" t="s">
         <v>56</v>
       </c>
@@ -1240,7 +1228,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="21" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="21" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E21" s="14" t="s">
         <v>58</v>
       </c>
@@ -1248,7 +1236,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E22" s="14" t="s">
         <v>60</v>
       </c>
@@ -1256,7 +1244,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="23" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="23" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E23" s="14" t="s">
         <v>62</v>
       </c>
@@ -1264,7 +1252,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="24" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="24" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E24" s="14" t="s">
         <v>64</v>
       </c>
@@ -1272,7 +1260,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E25" s="14" t="s">
         <v>66</v>
       </c>
@@ -1280,7 +1268,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E26" s="14" t="s">
         <v>44</v>
       </c>
@@ -1288,7 +1276,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E27" s="14" t="s">
         <v>69</v>
       </c>
@@ -1296,7 +1284,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="28" spans="5:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="5:6" x14ac:dyDescent="0.25">
       <c r="E28" s="14" t="s">
         <v>71</v>
       </c>
@@ -1312,36 +1300,36 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="5" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="2.44140625" style="5" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" style="5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="77.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="8.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.109375" style="5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="5" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="28" style="8" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="38.4" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:16" ht="38.25" x14ac:dyDescent="0.65">
       <c r="A1" s="5" t="s">
         <v>35</v>
       </c>
@@ -1359,7 +1347,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="50.4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="49.5" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>74</v>
       </c>
@@ -1403,7 +1391,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="str">
         <f>$A$1</f>
         <v>EC</v>
@@ -1416,7 +1404,7 @@
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15" t="s">
@@ -1436,12 +1424,12 @@
         <v>7</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="str">
         <f t="shared" ref="B5:B9" si="0">$A$1</f>
         <v>EC</v>
@@ -1454,7 +1442,7 @@
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="19" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15" t="s">
@@ -1474,12 +1462,12 @@
         <v>7</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="O5" s="18"/>
       <c r="P5" s="21"/>
     </row>
-    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -1492,7 +1480,7 @@
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="19" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15" t="s">
@@ -1512,12 +1500,12 @@
         <v>7</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="O6" s="18"/>
       <c r="P6" s="21"/>
     </row>
-    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -1530,7 +1518,7 @@
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="19" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G7" s="15"/>
       <c r="H7" s="15" t="s">
@@ -1545,15 +1533,15 @@
         <v>1</v>
       </c>
       <c r="M7" s="15" t="s">
-        <v>104</v>
+        <v>12</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="O7" s="18"/>
       <c r="P7" s="21"/>
     </row>
-    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -1575,7 +1563,7 @@
       <c r="O8" s="18"/>
       <c r="P8" s="21"/>
     </row>
-    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -1597,13 +1585,13 @@
       <c r="O9" s="18"/>
       <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:16" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:16" ht="25.5" x14ac:dyDescent="0.5">
       <c r="F11" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -1613,7 +1601,7 @@
       <c r="L12" s="25"/>
       <c r="M12" s="26"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
@@ -1623,7 +1611,7 @@
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
@@ -1633,7 +1621,7 @@
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
@@ -1656,31 +1644,31 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="5">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000000000000}">
           <x14:formula1>
             <xm:f>Instellingen!$B$2:$B$5</xm:f>
           </x14:formula1>
           <xm:sqref>D4:E9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000001000000}">
           <x14:formula1>
             <xm:f>Instellingen!$E$2:$E$27</xm:f>
           </x14:formula1>
           <xm:sqref>A1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000002000000}">
           <x14:formula1>
             <xm:f>Instellingen!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>K4:K9 M4:M9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000003000000}">
           <x14:formula1>
             <xm:f>Instellingen!$H$2:$H$6</xm:f>
           </x14:formula1>
           <xm:sqref>H4:H9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0100-000004000000}">
           <x14:formula1>
             <xm:f>Instellingen!$F$2:$F$27</xm:f>
           </x14:formula1>
@@ -1693,7 +1681,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -1703,26 +1691,26 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="5" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="2.44140625" style="5" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" style="5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="77.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="8.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.109375" style="5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="5" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="28" style="8" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="38.4" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:16" ht="38.25" x14ac:dyDescent="0.65">
       <c r="A1" s="5" t="str">
         <f>'4M PTA en programma'!A1</f>
         <v>EC</v>
@@ -1742,7 +1730,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="50.4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="49.5" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>74</v>
       </c>
@@ -1786,7 +1774,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="str">
         <f>$A$1</f>
         <v>EC</v>
@@ -1822,7 +1810,7 @@
       <c r="O4" s="18"/>
       <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="str">
         <f t="shared" ref="B5:B9" si="0">$A$1</f>
         <v>EC</v>
@@ -1857,12 +1845,12 @@
         <v>7</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="O5" s="18"/>
       <c r="P5" s="21"/>
     </row>
-    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -1875,7 +1863,7 @@
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G6" s="15">
         <v>1</v>
@@ -1897,12 +1885,12 @@
         <v>12</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="O6" s="18"/>
       <c r="P6" s="21"/>
     </row>
-    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -1938,7 +1926,7 @@
       <c r="O7" s="18"/>
       <c r="P7" s="21"/>
     </row>
-    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -1973,12 +1961,12 @@
         <v>7</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="O8" s="18"/>
       <c r="P8" s="21"/>
     </row>
-    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -2000,13 +1988,13 @@
       <c r="O9" s="18"/>
       <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:16" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:16" ht="25.5" x14ac:dyDescent="0.5">
       <c r="F11" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -2016,7 +2004,7 @@
       <c r="L12" s="25"/>
       <c r="M12" s="26"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
@@ -2026,7 +2014,7 @@
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
@@ -2036,7 +2024,7 @@
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
@@ -2059,25 +2047,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000000000000}">
           <x14:formula1>
             <xm:f>Instellingen!$H$2:$H$6</xm:f>
           </x14:formula1>
           <xm:sqref>H4:H9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>
             <xm:f>Instellingen!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>K4:K9 M4:M9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000002000000}">
           <x14:formula1>
             <xm:f>Instellingen!$E$2:$E$27</xm:f>
           </x14:formula1>
           <xm:sqref>A1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000003000000}">
           <x14:formula1>
             <xm:f>Instellingen!$B$2:$B$5</xm:f>
           </x14:formula1>
@@ -2090,7 +2078,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2100,26 +2088,26 @@
       <selection activeCell="N6" sqref="N6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="5" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="2.44140625" style="5" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" style="5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="77.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="8.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.109375" style="5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="5" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="28" style="8" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="38.4" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:16" ht="38.25" x14ac:dyDescent="0.65">
       <c r="A1" s="5" t="str">
         <f>'4M PTA en programma'!A1</f>
         <v>EC</v>
@@ -2139,7 +2127,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="50.4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="49.5" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>74</v>
       </c>
@@ -2183,7 +2171,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="str">
         <f>$A$1</f>
         <v>EC</v>
@@ -2216,12 +2204,12 @@
         <v>7</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="str">
         <f t="shared" ref="B5:B9" si="0">$A$1</f>
         <v>EC</v>
@@ -2254,12 +2242,12 @@
         <v>7</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="O5" s="18"/>
       <c r="P5" s="21"/>
     </row>
-    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -2292,12 +2280,12 @@
         <v>7</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="O6" s="18"/>
       <c r="P6" s="21"/>
     </row>
-    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -2319,7 +2307,7 @@
       <c r="O7" s="18"/>
       <c r="P7" s="21"/>
     </row>
-    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -2341,7 +2329,7 @@
       <c r="O8" s="18"/>
       <c r="P8" s="21"/>
     </row>
-    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -2363,13 +2351,13 @@
       <c r="O9" s="18"/>
       <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:16" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:16" ht="25.5" x14ac:dyDescent="0.5">
       <c r="F11" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -2379,7 +2367,7 @@
       <c r="L12" s="25"/>
       <c r="M12" s="26"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
@@ -2389,7 +2377,7 @@
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
@@ -2399,7 +2387,7 @@
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
@@ -2422,25 +2410,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000000000000}">
           <x14:formula1>
             <xm:f>Instellingen!$B$2:$B$5</xm:f>
           </x14:formula1>
           <xm:sqref>D4:E9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000001000000}">
           <x14:formula1>
             <xm:f>Instellingen!$E$2:$E$27</xm:f>
           </x14:formula1>
           <xm:sqref>A1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000002000000}">
           <x14:formula1>
             <xm:f>Instellingen!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>K4:K9 M4:M9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0300-000003000000}">
           <x14:formula1>
             <xm:f>Instellingen!$H$2:$H$6</xm:f>
           </x14:formula1>
@@ -2453,7 +2441,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2463,26 +2451,26 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="5" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="2.44140625" style="5" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" style="5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="77.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="8.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.109375" style="5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="5" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="28" style="8" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="38.4" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:16" ht="38.25" x14ac:dyDescent="0.65">
       <c r="A1" s="5" t="str">
         <f>'4M PTA en programma'!A1</f>
         <v>EC</v>
@@ -2502,7 +2490,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="50.4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="49.5" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>74</v>
       </c>
@@ -2546,7 +2534,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="str">
         <f>$A$1</f>
         <v>EC</v>
@@ -2582,7 +2570,7 @@
       <c r="O4" s="18"/>
       <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="str">
         <f t="shared" ref="B5:B9" si="0">$A$1</f>
         <v>EC</v>
@@ -2618,7 +2606,7 @@
       <c r="O5" s="18"/>
       <c r="P5" s="21"/>
     </row>
-    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -2631,7 +2619,7 @@
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="19" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G6" s="15">
         <v>1</v>
@@ -2654,7 +2642,7 @@
       <c r="O6" s="18"/>
       <c r="P6" s="21"/>
     </row>
-    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -2690,7 +2678,7 @@
       <c r="O7" s="18"/>
       <c r="P7" s="21"/>
     </row>
-    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -2712,7 +2700,7 @@
       <c r="O8" s="18"/>
       <c r="P8" s="21"/>
     </row>
-    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -2734,13 +2722,13 @@
       <c r="O9" s="18"/>
       <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:16" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:16" ht="25.5" x14ac:dyDescent="0.5">
       <c r="F11" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -2750,7 +2738,7 @@
       <c r="L12" s="25"/>
       <c r="M12" s="26"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
@@ -2760,7 +2748,7 @@
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
@@ -2770,7 +2758,7 @@
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
@@ -2793,25 +2781,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000000000000}">
           <x14:formula1>
             <xm:f>Instellingen!$H$2:$H$6</xm:f>
           </x14:formula1>
           <xm:sqref>H4:H9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000001000000}">
           <x14:formula1>
             <xm:f>Instellingen!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>K4:K9 M4:M9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000002000000}">
           <x14:formula1>
             <xm:f>Instellingen!$E$2:$E$27</xm:f>
           </x14:formula1>
           <xm:sqref>A1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0400-000003000000}">
           <x14:formula1>
             <xm:f>Instellingen!$B$2:$B$5</xm:f>
           </x14:formula1>
@@ -2824,7 +2812,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2834,26 +2822,26 @@
       <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="5" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="2.44140625" style="5" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" style="5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="77.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="8.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.109375" style="5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="5" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="28" style="8" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="38.4" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:16" ht="38.25" x14ac:dyDescent="0.65">
       <c r="A1" s="5" t="str">
         <f>'4M PTA en programma'!A1</f>
         <v>EC</v>
@@ -2873,7 +2861,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="50.4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="49.5" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>74</v>
       </c>
@@ -2917,7 +2905,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="str">
         <f>$A$1</f>
         <v>EC</v>
@@ -2952,12 +2940,12 @@
         <v>7</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="str">
         <f t="shared" ref="B5:B9" si="0">$A$1</f>
         <v>EC</v>
@@ -2990,12 +2978,12 @@
         <v>12</v>
       </c>
       <c r="N5" s="17" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="O5" s="18"/>
       <c r="P5" s="21"/>
     </row>
-    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -3030,12 +3018,12 @@
         <v>7</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="O6" s="18"/>
       <c r="P6" s="21"/>
     </row>
-    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -3048,7 +3036,7 @@
       </c>
       <c r="E7" s="16"/>
       <c r="F7" s="19" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G7" s="15">
         <v>1</v>
@@ -3068,12 +3056,12 @@
         <v>12</v>
       </c>
       <c r="N7" s="17" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="O7" s="18"/>
       <c r="P7" s="21"/>
     </row>
-    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -3108,12 +3096,12 @@
         <v>7</v>
       </c>
       <c r="N8" s="17" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="O8" s="18"/>
       <c r="P8" s="21"/>
     </row>
-    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -3135,13 +3123,13 @@
       <c r="O9" s="18"/>
       <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:16" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:16" ht="25.5" x14ac:dyDescent="0.5">
       <c r="F11" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -3151,7 +3139,7 @@
       <c r="L12" s="25"/>
       <c r="M12" s="26"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
@@ -3161,7 +3149,7 @@
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
@@ -3171,7 +3159,7 @@
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
@@ -3194,25 +3182,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000000000000}">
           <x14:formula1>
             <xm:f>Instellingen!$B$2:$B$5</xm:f>
           </x14:formula1>
           <xm:sqref>D4:E9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000001000000}">
           <x14:formula1>
             <xm:f>Instellingen!$E$2:$E$27</xm:f>
           </x14:formula1>
           <xm:sqref>A1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000002000000}">
           <x14:formula1>
             <xm:f>Instellingen!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>K4:K9 M4:M9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0500-000003000000}">
           <x14:formula1>
             <xm:f>Instellingen!$H$2:$H$6</xm:f>
           </x14:formula1>
@@ -3225,36 +3213,36 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:P15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="16.8" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="9.109375" style="5" hidden="1" customWidth="1"/>
-    <col min="2" max="2" width="2.44140625" style="5" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="2.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="5" hidden="1" customWidth="1"/>
+    <col min="2" max="2" width="2.42578125" style="5" hidden="1" customWidth="1"/>
+    <col min="3" max="3" width="2.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8" style="5" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="77.88671875" style="1" customWidth="1"/>
-    <col min="7" max="7" width="8.44140625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="8.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="77.85546875" style="1" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" style="1" customWidth="1"/>
+    <col min="8" max="8" width="8.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="8.44140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24.33203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="15.109375" style="5" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="8.42578125" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" style="1" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="5" hidden="1" customWidth="1"/>
     <col min="16" max="16" width="28" style="8" customWidth="1"/>
-    <col min="17" max="16384" width="9.109375" style="1"/>
+    <col min="17" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="38.4" x14ac:dyDescent="0.85">
+    <row r="1" spans="1:16" ht="38.25" x14ac:dyDescent="0.65">
       <c r="A1" s="5" t="str">
         <f>'4M PTA en programma'!A1</f>
         <v>EC</v>
@@ -3274,7 +3262,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:16" ht="50.4" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" ht="49.5" x14ac:dyDescent="0.3">
       <c r="C3" s="3" t="s">
         <v>74</v>
       </c>
@@ -3318,7 +3306,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="5" t="str">
         <f>$A$1</f>
         <v>EC</v>
@@ -3331,7 +3319,7 @@
       </c>
       <c r="E4" s="16"/>
       <c r="F4" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G4" s="15"/>
       <c r="H4" s="15" t="s">
@@ -3351,12 +3339,12 @@
         <v>7</v>
       </c>
       <c r="N4" s="17" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="O4" s="18"/>
       <c r="P4" s="21"/>
     </row>
-    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="5" t="str">
         <f t="shared" ref="B5:B9" si="0">$A$1</f>
         <v>EC</v>
@@ -3369,7 +3357,7 @@
       </c>
       <c r="E5" s="16"/>
       <c r="F5" s="19" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G5" s="15"/>
       <c r="H5" s="15" t="s">
@@ -3394,7 +3382,7 @@
       <c r="O5" s="18"/>
       <c r="P5" s="21"/>
     </row>
-    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -3407,7 +3395,7 @@
       </c>
       <c r="E6" s="16"/>
       <c r="F6" s="19" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G6" s="15"/>
       <c r="H6" s="15" t="s">
@@ -3427,12 +3415,12 @@
         <v>7</v>
       </c>
       <c r="N6" s="20" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="O6" s="18"/>
       <c r="P6" s="21"/>
     </row>
-    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -3454,7 +3442,7 @@
       <c r="O7" s="18"/>
       <c r="P7" s="21"/>
     </row>
-    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -3476,7 +3464,7 @@
       <c r="O8" s="18"/>
       <c r="P8" s="21"/>
     </row>
-    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="5" t="str">
         <f t="shared" si="0"/>
         <v>EC</v>
@@ -3498,13 +3486,13 @@
       <c r="O9" s="18"/>
       <c r="P9" s="21"/>
     </row>
-    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.4"/>
-    <row r="11" spans="1:16" ht="24.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:16" ht="7.5" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:16" ht="25.5" x14ac:dyDescent="0.5">
       <c r="F11" s="13" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" ht="100.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
       <c r="H12" s="25"/>
@@ -3514,7 +3502,7 @@
       <c r="L12" s="25"/>
       <c r="M12" s="26"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F13" s="27"/>
       <c r="G13" s="27"/>
       <c r="H13" s="27"/>
@@ -3524,7 +3512,7 @@
       <c r="L13" s="27"/>
       <c r="M13" s="27"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F14" s="27"/>
       <c r="G14" s="27"/>
       <c r="H14" s="27"/>
@@ -3534,7 +3522,7 @@
       <c r="L14" s="27"/>
       <c r="M14" s="27"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
       <c r="F15" s="27"/>
       <c r="G15" s="27"/>
       <c r="H15" s="27"/>
@@ -3557,25 +3545,25 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="4">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000000000000}">
           <x14:formula1>
             <xm:f>Instellingen!$H$2:$H$6</xm:f>
           </x14:formula1>
           <xm:sqref>H4:H9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000001000000}">
           <x14:formula1>
             <xm:f>Instellingen!$D$2:$D$3</xm:f>
           </x14:formula1>
           <xm:sqref>K4:K9 M4:M9</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000002000000}">
           <x14:formula1>
             <xm:f>Instellingen!$E$2:$E$27</xm:f>
           </x14:formula1>
           <xm:sqref>A1</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0600-000003000000}">
           <x14:formula1>
             <xm:f>Instellingen!$B$2:$B$5</xm:f>
           </x14:formula1>
@@ -3588,8 +3576,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016E4FC6D1D8BEB4897925B804975E464" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d1b9eb8218e1b9c44ac2e3457213f356">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="712ff825-c25b-4fa7-980d-494c05af82bb" xmlns:ns3="c6d635e9-0601-4b5e-ad25-fb7c8926c588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="a1a8fb4b100830f2cec8791afb97192b" ns2:_="" ns3:_="">
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010016E4FC6D1D8BEB4897925B804975E464" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2f4c844f49b69eee736f813a22d8de94">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="712ff825-c25b-4fa7-980d-494c05af82bb" xmlns:ns3="c6d635e9-0601-4b5e-ad25-fb7c8926c588" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f46293e76f6d1b28acbb6f6ff8d92fe2" ns2:_="" ns3:_="">
     <xsd:import namespace="712ff825-c25b-4fa7-980d-494c05af82bb"/>
     <xsd:import namespace="c6d635e9-0601-4b5e-ad25-fb7c8926c588"/>
     <xsd:element name="properties">
@@ -3602,6 +3599,13 @@
                 <xsd:element ref="ns2:MediaServiceFastMetadata" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithUsers" minOccurs="0"/>
                 <xsd:element ref="ns3:SharedWithDetails" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceAutoTags" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceOCR" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceGenerationTime" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceEventHashCode" minOccurs="0"/>
+                <xsd:element ref="ns2:MediaServiceDateTaken" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -3620,6 +3624,45 @@
     <xsd:element name="MediaServiceFastMetadata" ma:index="9" nillable="true" ma:displayName="MediaServiceFastMetadata" ma:hidden="true" ma:internalName="MediaServiceFastMetadata" ma:readOnly="true">
       <xsd:simpleType>
         <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoKeyPoints" ma:index="12" nillable="true" ma:displayName="MediaServiceAutoKeyPoints" ma:hidden="true" ma:internalName="MediaServiceAutoKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceKeyPoints" ma:index="13" nillable="true" ma:displayName="KeyPoints" ma:internalName="MediaServiceKeyPoints" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceAutoTags" ma:index="14" nillable="true" ma:displayName="Tags" ma:internalName="MediaServiceAutoTags" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceOCR" ma:index="15" nillable="true" ma:displayName="Extracted Text" ma:internalName="MediaServiceOCR" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Note">
+          <xsd:maxLength value="255"/>
+        </xsd:restriction>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceGenerationTime" ma:index="16" nillable="true" ma:displayName="MediaServiceGenerationTime" ma:hidden="true" ma:internalName="MediaServiceGenerationTime" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceEventHashCode" ma:index="17" nillable="true" ma:displayName="MediaServiceEventHashCode" ma:hidden="true" ma:internalName="MediaServiceEventHashCode" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceDateTaken" ma:index="18" nillable="true" ma:displayName="MediaServiceDateTaken" ma:hidden="true" ma:internalName="MediaServiceDateTaken" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
       </xsd:simpleType>
     </xsd:element>
   </xsd:schema>
@@ -3752,15 +3795,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3768,7 +3802,15 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D6484743-EFC8-4743-870B-5062D60012D5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46E12234-211F-473B-82BB-65CD0F3F06C3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6430044B-5AC2-4F3D-9EE0-04D7AA9B36DA}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
@@ -3782,14 +3824,6 @@
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{46E12234-211F-473B-82BB-65CD0F3F06C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>